<commit_message>
fix: filter sheets starting with underscore
</commit_message>
<xml_diff>
--- a/data/scenario-1-build.xlsx
+++ b/data/scenario-1-build.xlsx
@@ -5,11 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="init" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="sequence1" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="_flags" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="_params" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="_characters" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -93,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="389">
   <si>
     <t xml:space="preserve">Card Name</t>
   </si>
@@ -417,6 +420,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">intro_finish=true</t>
     </r>
@@ -989,32 +993,7 @@
     <t xml:space="preserve">Breakfast philosophy</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Daycycle=0-0,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">intro_finish=true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">;</t>
-    </r>
+    <t xml:space="preserve">Daycycle=0-0,intro_finish=true;</t>
   </si>
   <si>
     <t xml:space="preserve">There are so many conflicting parties in environmental politics. How should I convince my opposition?</t>
@@ -1051,16 +1030,269 @@
   </si>
   <si>
     <t xml:space="preserve">Stay on target. Focus on the environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windfarm_Built  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windfarm_Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ImportEng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind_Build_Coast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind_Build_Int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GreenEng_Req</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GreenEng_NotReq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windfarm_Tourism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windfarm_Subs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coast_Shallow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coast_Deep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windfarm_Fin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GreenEng_Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GreenEng_BizFirst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GreenEng_FamFirst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GreenEng_Incen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GreenEng_NoIncen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windfarm_Public</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windfarm_True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windfarm_Sale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windfarm_NoSale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seq1_Fin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GreenEng_Fin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrenEng_Shut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GreenEng_NoShut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">init</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intro_finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IconSize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Econ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GiNetworkBars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jobs and Economy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Envi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GiThreeLeaves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PopMiner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GiGoldMine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Popularity with Miners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PopUndec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GiBrainFreeze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Popularity with Undecided Voters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PopEnvi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GiSpotedFlower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Popularity with Environmentalist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Money</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GiMoneyStack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Budget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GreenEng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GiBoatPropeller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of province using green energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">daycycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">envira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1546541612-82d19b258cd5?fit=crop&amp;w=800&amp;q=60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">campaignAdvisor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1573497019940-1c28c88b4f3e?fit=crop&amp;w=800&amp;q=60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coalMiner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1529088746738-c4c0a152fb2c?fit=crop&amp;w=800&amp;q=60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">environmentallyMindedCitizen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">undecidedVoter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1584799235813-aaf50775698c?fit=crop&amp;w=800&amp;q=60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1529229089-f5719a804879?fit=crop&amp;w=800&amp;q=60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1548247416-ec66f4900b2e?fit=crop&amp;w=800&amp;q=60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1600187777399-220e82950adc?fit=crop&amp;w=800&amp;q=60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">powerplant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.pexels.com/photos/3044473/pexels-photo-3044473.jpeg?auto=compress&amp;cs=tinysrgb&amp;dpr=2&amp;h=300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1497435334941-8c899ee9e8e9?fit=crop&amp;w=800&amp;q=60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1602697245635-4e40e3bba87d?fit=crop&amp;w=800&amp;q=60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1621087955713-429347cb00e4?fit=crop&amp;w=800&amp;q=60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1614940873537-487b4741dbaa?fit=crop&amp;w=800&amp;q=60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1619275526612-bdaf4cd9bc9b?fit=crop&amp;w=800&amp;q=60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1536689423400-602247d31184?fit=crop&amp;w=800&amp;q=60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1557040135-9dc2a6b60411?fit=crop&amp;w=800&amp;q=60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1580411450318-6abb27b94eeb?fit=crop&amp;w=800&amp;q=60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1560250097-0b93528c311a?fit=crop&amp;w=800&amp;q=60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.unsplash.com/photo-1569032915512-922c2e506c51?fit=crop&amp;w=800&amp;q=60</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1126,16 +1358,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1159,13 +1386,8 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1182,6 +1404,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1234,7 +1462,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1275,11 +1503,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1287,12 +1515,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1378,11 +1614,11 @@
       <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="40.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.14"/>
   </cols>
@@ -2326,11 +2562,11 @@
   </sheetPr>
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G7" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O18" activeCellId="0" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.57"/>
@@ -2339,7 +2575,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="18.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="51.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="52.39"/>
   </cols>
@@ -2443,10 +2679,10 @@
       <c r="F3" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="5" t="s">
         <v>99</v>
       </c>
       <c r="I3" s="6" t="s">
@@ -2455,7 +2691,7 @@
       <c r="J3" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="10" t="s">
         <v>101</v>
       </c>
       <c r="N3" s="0" t="n">
@@ -2464,7 +2700,7 @@
       <c r="O3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="P3" s="12"/>
+      <c r="P3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="88.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
@@ -2485,10 +2721,10 @@
       <c r="F4" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="12" t="s">
         <v>107</v>
       </c>
       <c r="I4" s="6" t="s">
@@ -2497,14 +2733,14 @@
       <c r="J4" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>101</v>
       </c>
       <c r="N4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="O4" s="5"/>
-      <c r="P4" s="12"/>
+      <c r="P4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="25.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
@@ -2525,23 +2761,23 @@
       <c r="F5" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="10" t="s">
         <v>101</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="O5" s="5"/>
-      <c r="P5" s="12"/>
+      <c r="P5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="25.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>111</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2559,10 +2795,10 @@
       <c r="F6" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="12" t="s">
         <v>114</v>
       </c>
       <c r="I6" s="5" t="s">
@@ -2571,18 +2807,18 @@
       <c r="J6" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="10" t="s">
         <v>116</v>
       </c>
       <c r="N6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="O6" s="12" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="25.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>118</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -2600,10 +2836,10 @@
       <c r="F7" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="12" t="s">
         <v>121</v>
       </c>
       <c r="I7" s="5" t="s">
@@ -2612,13 +2848,13 @@
       <c r="J7" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="K7" s="10" t="s">
         <v>123</v>
       </c>
       <c r="N7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O7" s="13" t="s">
+      <c r="O7" s="12" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2649,13 +2885,13 @@
       <c r="J8" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="10" t="s">
         <v>126</v>
       </c>
       <c r="N8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O8" s="12"/>
+      <c r="O8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="25.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
@@ -2676,10 +2912,10 @@
       <c r="F9" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="12" t="s">
         <v>133</v>
       </c>
       <c r="I9" s="5" t="s">
@@ -2688,13 +2924,13 @@
       <c r="J9" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="10" t="s">
         <v>126</v>
       </c>
       <c r="N9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O9" s="12"/>
+      <c r="O9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="51.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
@@ -2715,10 +2951,10 @@
       <c r="F10" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="12" t="s">
         <v>141</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -2727,13 +2963,13 @@
       <c r="J10" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="10" t="s">
         <v>96</v>
       </c>
       <c r="N10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O10" s="12"/>
+      <c r="O10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="51.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
@@ -2754,19 +2990,19 @@
       <c r="F11" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="10" t="s">
         <v>17</v>
       </c>
       <c r="N11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O11" s="13" t="s">
+      <c r="O11" s="12" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2789,19 +3025,19 @@
       <c r="F12" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="10" t="s">
         <v>150</v>
       </c>
       <c r="N12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O12" s="13" t="s">
+      <c r="O12" s="12" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2824,19 +3060,19 @@
       <c r="F13" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="K13" s="10" t="s">
         <v>163</v>
       </c>
       <c r="N13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O13" s="13" t="s">
+      <c r="O13" s="12" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2859,19 +3095,19 @@
       <c r="F14" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K14" s="10" t="s">
         <v>150</v>
       </c>
       <c r="N14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O14" s="13" t="s">
+      <c r="O14" s="12" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2894,10 +3130,10 @@
       <c r="F15" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="12" t="s">
         <v>176</v>
       </c>
       <c r="I15" s="5" t="s">
@@ -2906,13 +3142,13 @@
       <c r="J15" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="K15" s="10" t="s">
         <v>96</v>
       </c>
       <c r="N15" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O15" s="13" t="s">
+      <c r="O15" s="12" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2935,19 +3171,19 @@
       <c r="F16" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="K16" s="11" t="s">
+      <c r="K16" s="10" t="s">
         <v>126</v>
       </c>
       <c r="N16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O16" s="13" t="s">
+      <c r="O16" s="12" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2961,28 +3197,28 @@
       <c r="C17" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>188</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="K17" s="11" t="s">
+      <c r="K17" s="10" t="s">
         <v>112</v>
       </c>
       <c r="N17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O17" s="13" t="s">
+      <c r="O17" s="12" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2996,7 +3232,7 @@
       <c r="C18" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>195</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -3005,19 +3241,19 @@
       <c r="F18" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="H18" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="K18" s="11" t="s">
+      <c r="K18" s="10" t="s">
         <v>119</v>
       </c>
       <c r="N18" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O18" s="13" t="s">
+      <c r="O18" s="12" t="s">
         <v>200</v>
       </c>
     </row>
@@ -3031,7 +3267,7 @@
       <c r="C19" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>201</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -3040,10 +3276,10 @@
       <c r="F19" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="12" t="s">
         <v>205</v>
       </c>
       <c r="I19" s="5" t="s">
@@ -3052,13 +3288,13 @@
       <c r="J19" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="K19" s="11" t="s">
+      <c r="K19" s="10" t="s">
         <v>207</v>
       </c>
       <c r="N19" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O19" s="13" t="s">
+      <c r="O19" s="12" t="s">
         <v>208</v>
       </c>
     </row>
@@ -3081,10 +3317,10 @@
       <c r="F20" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="12" t="s">
         <v>213</v>
       </c>
       <c r="I20" s="5" t="s">
@@ -3093,18 +3329,18 @@
       <c r="J20" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="K20" s="11" t="s">
+      <c r="K20" s="10" t="s">
         <v>214</v>
       </c>
       <c r="N20" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O20" s="13" t="s">
+      <c r="O20" s="12" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="51.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>216</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -3122,10 +3358,10 @@
       <c r="F21" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="12" t="s">
         <v>222</v>
       </c>
       <c r="I21" s="5" t="s">
@@ -3134,18 +3370,18 @@
       <c r="J21" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="K21" s="11" t="s">
+      <c r="K21" s="10" t="s">
         <v>217</v>
       </c>
       <c r="N21" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O21" s="13" t="s">
+      <c r="O21" s="12" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="51.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="13" t="s">
         <v>224</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -3163,10 +3399,10 @@
       <c r="F22" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="H22" s="13" t="s">
+      <c r="H22" s="12" t="s">
         <v>230</v>
       </c>
       <c r="I22" s="5" t="s">
@@ -3175,13 +3411,13 @@
       <c r="J22" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="K22" s="11" t="s">
+      <c r="K22" s="10" t="s">
         <v>225</v>
       </c>
       <c r="N22" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O22" s="13" t="s">
+      <c r="O22" s="12" t="s">
         <v>231</v>
       </c>
     </row>
@@ -3204,10 +3440,10 @@
       <c r="F23" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="H23" s="12" t="s">
         <v>237</v>
       </c>
       <c r="I23" s="5" t="s">
@@ -3216,13 +3452,13 @@
       <c r="J23" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="K23" s="11" t="s">
+      <c r="K23" s="10" t="s">
         <v>17</v>
       </c>
       <c r="N23" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O23" s="13" t="s">
+      <c r="O23" s="12" t="s">
         <v>239</v>
       </c>
     </row>
@@ -3245,10 +3481,10 @@
       <c r="F24" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="12" t="s">
         <v>245</v>
       </c>
       <c r="I24" s="5" t="s">
@@ -3257,13 +3493,13 @@
       <c r="J24" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="K24" s="11" t="s">
+      <c r="K24" s="10" t="s">
         <v>17</v>
       </c>
       <c r="N24" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O24" s="13" t="s">
+      <c r="O24" s="12" t="s">
         <v>246</v>
       </c>
     </row>
@@ -3286,10 +3522,10 @@
       <c r="F25" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="G25" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="H25" s="13" t="s">
+      <c r="H25" s="12" t="s">
         <v>252</v>
       </c>
       <c r="I25" s="5" t="s">
@@ -3298,13 +3534,13 @@
       <c r="J25" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="K25" s="11" t="s">
+      <c r="K25" s="10" t="s">
         <v>157</v>
       </c>
       <c r="N25" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O25" s="13" t="s">
+      <c r="O25" s="12" t="s">
         <v>253</v>
       </c>
     </row>
@@ -3327,10 +3563,10 @@
       <c r="F26" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="G26" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="H26" s="12" t="s">
         <v>258</v>
       </c>
       <c r="I26" s="5" t="s">
@@ -3339,11 +3575,11 @@
       <c r="J26" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="K26" s="11"/>
+      <c r="K26" s="10"/>
       <c r="N26" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O26" s="13" t="s">
+      <c r="O26" s="12" t="s">
         <v>259</v>
       </c>
     </row>
@@ -3360,16 +3596,16 @@
       <c r="D27" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="12" t="s">
         <v>261</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="12" t="s">
         <v>264</v>
       </c>
       <c r="I27" s="5" t="s">
@@ -3378,7 +3614,7 @@
       <c r="J27" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="K27" s="11" t="s">
+      <c r="K27" s="10" t="s">
         <v>112</v>
       </c>
       <c r="N27" s="0" t="n">
@@ -3398,7 +3634,7 @@
       <c r="C28" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="12" t="s">
         <v>268</v>
       </c>
       <c r="E28" s="5" t="s">
@@ -3407,13 +3643,13 @@
       <c r="F28" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="12" t="s">
         <v>271</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H28" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="K28" s="11" t="s">
+      <c r="K28" s="10" t="s">
         <v>96</v>
       </c>
       <c r="N28" s="0" t="n">
@@ -3439,19 +3675,19 @@
       <c r="F29" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G29" s="13" t="s">
+      <c r="G29" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="K29" s="11" t="s">
+      <c r="K29" s="10" t="s">
         <v>112</v>
       </c>
       <c r="N29" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O29" s="13" t="s">
+      <c r="O29" s="12" t="s">
         <v>275</v>
       </c>
     </row>
@@ -3474,19 +3710,19 @@
       <c r="F30" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G30" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="H30" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="K30" s="11" t="s">
+      <c r="K30" s="10" t="s">
         <v>96</v>
       </c>
       <c r="N30" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O30" s="13" t="s">
+      <c r="O30" s="12" t="s">
         <v>277</v>
       </c>
     </row>
@@ -3509,19 +3745,19 @@
       <c r="F31" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="G31" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="H31" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="K31" s="11" t="s">
+      <c r="K31" s="10" t="s">
         <v>112</v>
       </c>
       <c r="N31" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O31" s="13" t="s">
+      <c r="O31" s="12" t="s">
         <v>280</v>
       </c>
     </row>
@@ -3544,19 +3780,19 @@
       <c r="F32" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="G32" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="H32" s="13" t="s">
+      <c r="H32" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="K32" s="11" t="s">
+      <c r="K32" s="10" t="s">
         <v>96</v>
       </c>
       <c r="N32" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O32" s="13" t="s">
+      <c r="O32" s="12" t="s">
         <v>283</v>
       </c>
     </row>
@@ -3754,4 +3990,685 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.28"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="B3" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="B4" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="B5" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="B6" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="B7" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="B8" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="B9" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="B10" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="B11" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="B12" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="B13" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="B14" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="B15" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="B16" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="B17" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="B18" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="B19" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="B20" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="B21" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="B22" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="B23" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="B24" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="B25" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="B26" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B27" s="16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="B28" s="16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="56.69"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="142.42"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>388</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>